<commit_message>
save move html info out, with model + info pattern
</commit_message>
<xml_diff>
--- a/yxcfidc/data/meta/ct.xlsx
+++ b/yxcfidc/data/meta/ct.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>locId</t>
   </si>
@@ -146,6 +146,14 @@
   </si>
   <si>
     <t>data/ct/CT_KT_1/files.html</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>model</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>data/model/ct.html</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1064,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1075,12 +1083,13 @@
     <col min="2" max="2" width="14.125" customWidth="1"/>
     <col min="4" max="4" width="34.125" customWidth="1"/>
     <col min="5" max="5" width="15.625" customWidth="1"/>
-    <col min="7" max="7" width="28.625" customWidth="1"/>
-    <col min="8" max="8" width="28.25" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="7" max="7" width="28.75" customWidth="1"/>
+    <col min="8" max="8" width="28.625" customWidth="1"/>
+    <col min="9" max="9" width="28.25" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1100,16 +1109,19 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1129,16 +1141,19 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1158,16 +1173,19 @@
         <v>23</v>
       </c>
       <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>29</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1187,12 +1205,15 @@
         <v>24</v>
       </c>
       <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>35</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>